<commit_message>
route concept id handling
Former-commit-id: 61e1d5c04fdc1797994b7535a32835181bb874ae
</commit_message>
<xml_diff>
--- a/patient_addition/data.xlsx
+++ b/patient_addition/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\iDIA_Rules\patient_addition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erc53/Github/iDiA_Rules_EC/patient_addition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E6D8B2-291A-45EA-88F2-2C134D750398}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD534DB7-7279-644C-83E7-6372BECF65C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="1580" windowWidth="27980" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="27">
   <si>
     <t>INSERT_TYPE</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>ROUTE_ID</t>
   </si>
 </sst>
 </file>
@@ -647,24 +650,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -974,15 +960,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O481"/>
+  <dimension ref="A1:P487"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A461" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N487" sqref="N487"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1028,8 +1015,11 @@
       <c r="O1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1047,7 +1037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1067,7 +1057,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1087,7 +1077,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1107,7 +1097,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1127,7 +1117,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1159,7 +1149,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1191,7 +1181,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1223,7 +1213,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1244,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1264,7 +1254,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1284,7 +1274,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1304,7 +1294,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1324,7 +1314,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1356,7 +1346,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1388,7 +1378,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1409,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1429,7 +1419,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1449,7 +1439,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1469,7 +1459,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -1489,7 +1479,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1521,7 +1511,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1553,7 +1543,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1585,7 +1575,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1606,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1626,7 +1616,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1646,7 +1636,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1666,7 +1656,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1686,7 +1676,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1718,7 +1708,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1750,7 +1740,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -1782,7 +1772,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -1803,7 +1793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -1823,7 +1813,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -1843,7 +1833,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1863,7 +1853,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -1895,7 +1885,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1927,7 +1917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -1945,7 +1935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -1965,7 +1955,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -1985,7 +1975,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -2005,7 +1995,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -2037,7 +2027,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -2069,7 +2059,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -2092,7 +2082,7 @@
         <v>9557</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -2110,7 +2100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -2130,7 +2120,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -2150,7 +2140,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -2170,7 +2160,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -2190,7 +2180,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -2222,7 +2212,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -2254,7 +2244,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -2286,7 +2276,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -2309,7 +2299,7 @@
         <v>9557</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -2327,7 +2317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -2347,7 +2337,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -2367,7 +2357,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -2387,7 +2377,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -2419,7 +2409,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>16</v>
       </c>
@@ -2451,7 +2441,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -2474,7 +2464,7 @@
         <v>9557</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>18</v>
       </c>
@@ -2497,7 +2487,7 @@
         <v>8795</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -2515,7 +2505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -2535,7 +2525,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -2555,7 +2545,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -2575,7 +2565,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -2607,7 +2597,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -2639,7 +2629,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>18</v>
       </c>
@@ -2662,7 +2652,7 @@
         <v>9557</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>18</v>
       </c>
@@ -2685,7 +2675,7 @@
         <v>8795</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -2703,7 +2693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -2723,7 +2713,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>15</v>
       </c>
@@ -2743,7 +2733,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -2763,7 +2753,7 @@
         <v>9202</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -2795,7 +2785,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>16</v>
       </c>
@@ -2827,7 +2817,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>13</v>
       </c>
@@ -2845,7 +2835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -2865,7 +2855,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -2885,7 +2875,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -2905,7 +2895,7 @@
         <v>9202</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -2937,7 +2927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -2969,7 +2959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>13</v>
       </c>
@@ -2987,7 +2977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>15</v>
       </c>
@@ -3007,7 +2997,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -3027,7 +3017,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -3047,7 +3037,7 @@
         <v>9202</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -3079,7 +3069,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>16</v>
       </c>
@@ -3111,7 +3101,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>13</v>
       </c>
@@ -3129,7 +3119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>15</v>
       </c>
@@ -3149,7 +3139,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>15</v>
       </c>
@@ -3169,7 +3159,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -3189,7 +3179,7 @@
         <v>9202</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>16</v>
       </c>
@@ -3221,7 +3211,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>16</v>
       </c>
@@ -3253,7 +3243,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>13</v>
       </c>
@@ -3271,7 +3261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>15</v>
       </c>
@@ -3291,7 +3281,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>15</v>
       </c>
@@ -3311,7 +3301,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>14</v>
       </c>
@@ -3331,7 +3321,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>16</v>
       </c>
@@ -3363,7 +3353,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -3395,7 +3385,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>13</v>
       </c>
@@ -3413,7 +3403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>15</v>
       </c>
@@ -3433,7 +3423,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>15</v>
       </c>
@@ -3453,7 +3443,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>14</v>
       </c>
@@ -3473,7 +3463,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>16</v>
       </c>
@@ -3505,7 +3495,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>16</v>
       </c>
@@ -3537,7 +3527,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>13</v>
       </c>
@@ -3555,7 +3545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>15</v>
       </c>
@@ -3575,7 +3565,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>15</v>
       </c>
@@ -3595,7 +3585,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>14</v>
       </c>
@@ -3615,7 +3605,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>16</v>
       </c>
@@ -3647,7 +3637,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>16</v>
       </c>
@@ -3679,7 +3669,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>13</v>
       </c>
@@ -3697,7 +3687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>15</v>
       </c>
@@ -3717,7 +3707,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>15</v>
       </c>
@@ -3737,7 +3727,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>14</v>
       </c>
@@ -3757,7 +3747,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>16</v>
       </c>
@@ -3789,7 +3779,7 @@
         <v>4340851</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>16</v>
       </c>
@@ -3821,7 +3811,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>18</v>
       </c>
@@ -3844,7 +3834,7 @@
         <v>8795</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>13</v>
       </c>
@@ -3862,7 +3852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>15</v>
       </c>
@@ -3882,7 +3872,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>15</v>
       </c>
@@ -3902,7 +3892,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>14</v>
       </c>
@@ -3922,7 +3912,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>16</v>
       </c>
@@ -3954,7 +3944,7 @@
         <v>4340851</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>16</v>
       </c>
@@ -3986,7 +3976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>18</v>
       </c>
@@ -4009,7 +3999,7 @@
         <v>8795</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>13</v>
       </c>
@@ -4027,7 +4017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>15</v>
       </c>
@@ -4047,7 +4037,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>15</v>
       </c>
@@ -4067,7 +4057,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>14</v>
       </c>
@@ -4087,7 +4077,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>16</v>
       </c>
@@ -4119,7 +4109,7 @@
         <v>4340851</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>16</v>
       </c>
@@ -4151,7 +4141,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>18</v>
       </c>
@@ -4174,7 +4164,7 @@
         <v>8795</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>13</v>
       </c>
@@ -4192,7 +4182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>15</v>
       </c>
@@ -4212,7 +4202,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>15</v>
       </c>
@@ -4232,7 +4222,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>14</v>
       </c>
@@ -4252,7 +4242,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>16</v>
       </c>
@@ -4284,7 +4274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>16</v>
       </c>
@@ -4316,7 +4306,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>18</v>
       </c>
@@ -4339,7 +4329,7 @@
         <v>8795</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>13</v>
       </c>
@@ -4357,7 +4347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>15</v>
       </c>
@@ -4377,7 +4367,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>15</v>
       </c>
@@ -4397,7 +4387,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>14</v>
       </c>
@@ -4417,7 +4407,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>16</v>
       </c>
@@ -4449,7 +4439,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>16</v>
       </c>
@@ -4481,7 +4471,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>13</v>
       </c>
@@ -4499,7 +4489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>15</v>
       </c>
@@ -4519,7 +4509,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>15</v>
       </c>
@@ -4539,7 +4529,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>14</v>
       </c>
@@ -4559,7 +4549,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>16</v>
       </c>
@@ -4591,7 +4581,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>16</v>
       </c>
@@ -4623,7 +4613,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>13</v>
       </c>
@@ -4641,7 +4631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>15</v>
       </c>
@@ -4661,7 +4651,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>15</v>
       </c>
@@ -4681,7 +4671,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>15</v>
       </c>
@@ -4701,7 +4691,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>14</v>
       </c>
@@ -4721,7 +4711,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>16</v>
       </c>
@@ -4753,7 +4743,7 @@
         <v>4340851</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>16</v>
       </c>
@@ -4785,7 +4775,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>16</v>
       </c>
@@ -4817,7 +4807,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>13</v>
       </c>
@@ -4835,7 +4825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>15</v>
       </c>
@@ -4855,7 +4845,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>15</v>
       </c>
@@ -4875,7 +4865,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>14</v>
       </c>
@@ -4895,7 +4885,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>16</v>
       </c>
@@ -4927,7 +4917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>16</v>
       </c>
@@ -4959,7 +4949,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>13</v>
       </c>
@@ -4977,7 +4967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>15</v>
       </c>
@@ -4997,7 +4987,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>15</v>
       </c>
@@ -5017,7 +5007,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>15</v>
       </c>
@@ -5037,7 +5027,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>14</v>
       </c>
@@ -5057,7 +5047,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>16</v>
       </c>
@@ -5089,7 +5079,7 @@
         <v>4340851</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>16</v>
       </c>
@@ -5121,7 +5111,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>16</v>
       </c>
@@ -5153,7 +5143,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>13</v>
       </c>
@@ -5171,7 +5161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>15</v>
       </c>
@@ -5191,7 +5181,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>15</v>
       </c>
@@ -5211,7 +5201,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>15</v>
       </c>
@@ -5231,7 +5221,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>14</v>
       </c>
@@ -5251,7 +5241,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>16</v>
       </c>
@@ -5283,7 +5273,7 @@
         <v>4340851</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>16</v>
       </c>
@@ -5314,8 +5304,11 @@
       <c r="O181" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P181">
+        <v>4184451</v>
+      </c>
+    </row>
+    <row r="182" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>16</v>
       </c>
@@ -5347,7 +5340,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>13</v>
       </c>
@@ -5365,7 +5358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>15</v>
       </c>
@@ -5385,7 +5378,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>15</v>
       </c>
@@ -5405,7 +5398,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>14</v>
       </c>
@@ -5425,7 +5418,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>16</v>
       </c>
@@ -5457,7 +5450,7 @@
         <v>4340851</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>16</v>
       </c>
@@ -5488,8 +5481,11 @@
       <c r="O188" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P188">
+        <v>4184451</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>13</v>
       </c>
@@ -5507,7 +5503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>15</v>
       </c>
@@ -5527,7 +5523,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>15</v>
       </c>
@@ -5547,7 +5543,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>14</v>
       </c>
@@ -5567,7 +5563,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>16</v>
       </c>
@@ -5599,7 +5595,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>16</v>
       </c>
@@ -5631,7 +5627,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>13</v>
       </c>
@@ -5649,7 +5645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>15</v>
       </c>
@@ -5669,7 +5665,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>15</v>
       </c>
@@ -5689,7 +5685,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>14</v>
       </c>
@@ -5709,7 +5705,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>16</v>
       </c>
@@ -5741,7 +5737,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>16</v>
       </c>
@@ -5773,7 +5769,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>13</v>
       </c>
@@ -5791,7 +5787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>15</v>
       </c>
@@ -5811,7 +5807,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>15</v>
       </c>
@@ -5831,7 +5827,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>14</v>
       </c>
@@ -5851,7 +5847,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>16</v>
       </c>
@@ -5883,7 +5879,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>16</v>
       </c>
@@ -5915,7 +5911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>13</v>
       </c>
@@ -5933,7 +5929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>15</v>
       </c>
@@ -5953,7 +5949,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>15</v>
       </c>
@@ -5973,7 +5969,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>14</v>
       </c>
@@ -5993,7 +5989,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>16</v>
       </c>
@@ -6025,7 +6021,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>16</v>
       </c>
@@ -6057,7 +6053,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>13</v>
       </c>
@@ -6075,7 +6071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>15</v>
       </c>
@@ -6095,7 +6091,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>15</v>
       </c>
@@ -6115,7 +6111,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>15</v>
       </c>
@@ -6135,7 +6131,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>14</v>
       </c>
@@ -6155,7 +6151,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>16</v>
       </c>
@@ -6187,7 +6183,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>16</v>
       </c>
@@ -6219,7 +6215,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>16</v>
       </c>
@@ -6251,7 +6247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>13</v>
       </c>
@@ -6269,7 +6265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>15</v>
       </c>
@@ -6289,7 +6285,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>15</v>
       </c>
@@ -6309,7 +6305,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>15</v>
       </c>
@@ -6329,7 +6325,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>15</v>
       </c>
@@ -6349,7 +6345,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>14</v>
       </c>
@@ -6369,7 +6365,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>16</v>
       </c>
@@ -6401,7 +6397,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>16</v>
       </c>
@@ -6433,7 +6429,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>16</v>
       </c>
@@ -6465,7 +6461,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>16</v>
       </c>
@@ -6497,7 +6493,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>13</v>
       </c>
@@ -6515,7 +6511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>15</v>
       </c>
@@ -6535,7 +6531,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>15</v>
       </c>
@@ -6555,7 +6551,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>17</v>
       </c>
@@ -6575,7 +6571,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>14</v>
       </c>
@@ -6595,7 +6591,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="236" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>16</v>
       </c>
@@ -6627,7 +6623,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>16</v>
       </c>
@@ -6659,7 +6655,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="238" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>13</v>
       </c>
@@ -6677,7 +6673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>15</v>
       </c>
@@ -6697,7 +6693,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>15</v>
       </c>
@@ -6717,7 +6713,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>14</v>
       </c>
@@ -6737,7 +6733,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>16</v>
       </c>
@@ -6769,7 +6765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>16</v>
       </c>
@@ -6801,7 +6797,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>13</v>
       </c>
@@ -6819,7 +6815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>15</v>
       </c>
@@ -6839,7 +6835,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>15</v>
       </c>
@@ -6859,7 +6855,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>14</v>
       </c>
@@ -6879,7 +6875,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>16</v>
       </c>
@@ -6911,7 +6907,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>16</v>
       </c>
@@ -6943,7 +6939,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>13</v>
       </c>
@@ -6961,7 +6957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>15</v>
       </c>
@@ -6981,7 +6977,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>15</v>
       </c>
@@ -7001,7 +6997,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>14</v>
       </c>
@@ -7021,7 +7017,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>16</v>
       </c>
@@ -7053,7 +7049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>16</v>
       </c>
@@ -7085,7 +7081,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>13</v>
       </c>
@@ -7103,7 +7099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>15</v>
       </c>
@@ -7123,7 +7119,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="258" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>15</v>
       </c>
@@ -7143,7 +7139,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="259" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>15</v>
       </c>
@@ -7163,7 +7159,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="260" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>14</v>
       </c>
@@ -7183,7 +7179,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="261" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>16</v>
       </c>
@@ -7215,7 +7211,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="262" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>16</v>
       </c>
@@ -7247,7 +7243,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="263" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>16</v>
       </c>
@@ -7279,7 +7275,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="264" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>13</v>
       </c>
@@ -7297,7 +7293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>15</v>
       </c>
@@ -7317,7 +7313,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="266" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>15</v>
       </c>
@@ -7337,7 +7333,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="267" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>17</v>
       </c>
@@ -7357,7 +7353,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="268" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>14</v>
       </c>
@@ -7377,7 +7373,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="269" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>16</v>
       </c>
@@ -7409,7 +7405,7 @@
         <v>4340851</v>
       </c>
     </row>
-    <row r="270" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>16</v>
       </c>
@@ -7440,8 +7436,11 @@
       <c r="O270" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="271" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P270">
+        <v>4184451</v>
+      </c>
+    </row>
+    <row r="271" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>13</v>
       </c>
@@ -7459,7 +7458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>15</v>
       </c>
@@ -7479,7 +7478,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="273" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>15</v>
       </c>
@@ -7499,7 +7498,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="274" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>17</v>
       </c>
@@ -7519,7 +7518,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="275" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>14</v>
       </c>
@@ -7539,7 +7538,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="276" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>16</v>
       </c>
@@ -7571,7 +7570,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="277" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>16</v>
       </c>
@@ -7603,7 +7602,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="278" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>13</v>
       </c>
@@ -7621,7 +7620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>15</v>
       </c>
@@ -7641,7 +7640,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="280" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>15</v>
       </c>
@@ -7661,7 +7660,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="281" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>17</v>
       </c>
@@ -7681,7 +7680,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="282" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>14</v>
       </c>
@@ -7701,7 +7700,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="283" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>16</v>
       </c>
@@ -7733,7 +7732,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="284" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>16</v>
       </c>
@@ -7765,7 +7764,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="285" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>13</v>
       </c>
@@ -7783,7 +7782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="286" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>15</v>
       </c>
@@ -7803,7 +7802,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="287" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>15</v>
       </c>
@@ -7823,7 +7822,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="288" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>14</v>
       </c>
@@ -7843,7 +7842,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="289" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>16</v>
       </c>
@@ -7875,7 +7874,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="290" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>16</v>
       </c>
@@ -7907,7 +7906,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="291" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>13</v>
       </c>
@@ -7925,7 +7924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="292" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>15</v>
       </c>
@@ -7945,7 +7944,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="293" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>15</v>
       </c>
@@ -7965,7 +7964,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="294" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>14</v>
       </c>
@@ -7985,7 +7984,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="295" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>16</v>
       </c>
@@ -8017,7 +8016,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="296" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>16</v>
       </c>
@@ -8049,7 +8048,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="297" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>13</v>
       </c>
@@ -8067,7 +8066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>15</v>
       </c>
@@ -8087,7 +8086,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="299" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>15</v>
       </c>
@@ -8107,7 +8106,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="300" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>14</v>
       </c>
@@ -8127,7 +8126,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="301" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>16</v>
       </c>
@@ -8159,7 +8158,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="302" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>16</v>
       </c>
@@ -8191,7 +8190,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="303" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>13</v>
       </c>
@@ -8209,7 +8208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>15</v>
       </c>
@@ -8229,7 +8228,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="305" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>15</v>
       </c>
@@ -8249,7 +8248,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="306" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>14</v>
       </c>
@@ -8269,7 +8268,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="307" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>16</v>
       </c>
@@ -8301,7 +8300,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="308" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>16</v>
       </c>
@@ -8333,7 +8332,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="309" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>13</v>
       </c>
@@ -8351,7 +8350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>15</v>
       </c>
@@ -8371,7 +8370,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="311" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>15</v>
       </c>
@@ -8391,7 +8390,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="312" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>14</v>
       </c>
@@ -8411,7 +8410,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="313" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>16</v>
       </c>
@@ -8443,7 +8442,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="314" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>16</v>
       </c>
@@ -8475,7 +8474,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="315" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>13</v>
       </c>
@@ -8493,7 +8492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>15</v>
       </c>
@@ -8513,7 +8512,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="317" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>15</v>
       </c>
@@ -8533,7 +8532,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="318" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>14</v>
       </c>
@@ -8553,7 +8552,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="319" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>16</v>
       </c>
@@ -8585,7 +8584,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="320" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>16</v>
       </c>
@@ -8617,7 +8616,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="321" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>13</v>
       </c>
@@ -8635,7 +8634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>15</v>
       </c>
@@ -8655,7 +8654,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="323" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>15</v>
       </c>
@@ -8675,7 +8674,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="324" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>14</v>
       </c>
@@ -8695,7 +8694,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="325" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>16</v>
       </c>
@@ -8727,7 +8726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="326" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>16</v>
       </c>
@@ -8759,7 +8758,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="327" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>13</v>
       </c>
@@ -8777,7 +8776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>15</v>
       </c>
@@ -8797,7 +8796,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="329" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>15</v>
       </c>
@@ -8817,7 +8816,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="330" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>14</v>
       </c>
@@ -8837,7 +8836,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="331" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>16</v>
       </c>
@@ -8869,7 +8868,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="332" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>16</v>
       </c>
@@ -8901,7 +8900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="333" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>13</v>
       </c>
@@ -8919,7 +8918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>15</v>
       </c>
@@ -8939,7 +8938,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="335" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>15</v>
       </c>
@@ -8959,7 +8958,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="336" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>14</v>
       </c>
@@ -8979,7 +8978,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="337" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>16</v>
       </c>
@@ -9011,7 +9010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="338" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>16</v>
       </c>
@@ -9043,7 +9042,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="339" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>18</v>
       </c>
@@ -9066,7 +9065,7 @@
         <v>9557</v>
       </c>
     </row>
-    <row r="340" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>13</v>
       </c>
@@ -9084,7 +9083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>15</v>
       </c>
@@ -9104,7 +9103,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="342" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>15</v>
       </c>
@@ -9124,7 +9123,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="343" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>14</v>
       </c>
@@ -9144,7 +9143,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="344" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>16</v>
       </c>
@@ -9176,7 +9175,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="345" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>16</v>
       </c>
@@ -9208,7 +9207,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="346" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>13</v>
       </c>
@@ -9226,7 +9225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>15</v>
       </c>
@@ -9246,7 +9245,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="348" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>15</v>
       </c>
@@ -9266,7 +9265,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="349" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>15</v>
       </c>
@@ -9286,7 +9285,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="350" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>14</v>
       </c>
@@ -9306,7 +9305,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="351" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>16</v>
       </c>
@@ -9338,7 +9337,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="352" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>16</v>
       </c>
@@ -9369,8 +9368,11 @@
       <c r="O352" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="353" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P352">
+        <v>4184451</v>
+      </c>
+    </row>
+    <row r="353" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>16</v>
       </c>
@@ -9402,7 +9404,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="354" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>13</v>
       </c>
@@ -9420,7 +9422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>15</v>
       </c>
@@ -9440,7 +9442,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="356" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>15</v>
       </c>
@@ -9460,7 +9462,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="357" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>14</v>
       </c>
@@ -9480,7 +9482,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="358" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>16</v>
       </c>
@@ -9512,7 +9514,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="359" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>16</v>
       </c>
@@ -9543,8 +9545,11 @@
       <c r="O359" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="360" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P359">
+        <v>4184451</v>
+      </c>
+    </row>
+    <row r="360" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>13</v>
       </c>
@@ -9562,7 +9567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>15</v>
       </c>
@@ -9582,7 +9587,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="362" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>15</v>
       </c>
@@ -9602,7 +9607,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="363" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>17</v>
       </c>
@@ -9622,7 +9627,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="364" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>14</v>
       </c>
@@ -9642,7 +9647,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="365" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>16</v>
       </c>
@@ -9674,7 +9679,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="366" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>16</v>
       </c>
@@ -9705,8 +9710,11 @@
       <c r="O366" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="367" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P366">
+        <v>4184451</v>
+      </c>
+    </row>
+    <row r="367" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>13</v>
       </c>
@@ -9724,7 +9732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>15</v>
       </c>
@@ -9744,7 +9752,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="369" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>15</v>
       </c>
@@ -9764,7 +9772,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="370" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>14</v>
       </c>
@@ -9784,7 +9792,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="371" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>16</v>
       </c>
@@ -9816,7 +9824,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="372" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>16</v>
       </c>
@@ -9848,7 +9856,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="373" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>13</v>
       </c>
@@ -9866,7 +9874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>15</v>
       </c>
@@ -9886,7 +9894,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="375" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>15</v>
       </c>
@@ -9906,7 +9914,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="376" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>15</v>
       </c>
@@ -9926,7 +9934,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="377" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>14</v>
       </c>
@@ -9946,7 +9954,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="378" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>16</v>
       </c>
@@ -9978,7 +9986,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="379" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>16</v>
       </c>
@@ -10010,7 +10018,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="380" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>16</v>
       </c>
@@ -10042,7 +10050,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="381" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>13</v>
       </c>
@@ -10060,7 +10068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>15</v>
       </c>
@@ -10080,7 +10088,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="383" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>15</v>
       </c>
@@ -10100,7 +10108,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="384" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>17</v>
       </c>
@@ -10120,7 +10128,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="385" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>14</v>
       </c>
@@ -10140,7 +10148,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="386" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>16</v>
       </c>
@@ -10172,7 +10180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="387" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>16</v>
       </c>
@@ -10204,7 +10212,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="388" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>13</v>
       </c>
@@ -10222,7 +10230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="389" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>15</v>
       </c>
@@ -10242,7 +10250,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="390" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>15</v>
       </c>
@@ -10262,7 +10270,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="391" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>14</v>
       </c>
@@ -10282,7 +10290,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="392" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>16</v>
       </c>
@@ -10314,7 +10322,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="393" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>16</v>
       </c>
@@ -10346,7 +10354,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="394" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>13</v>
       </c>
@@ -10364,7 +10372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="395" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>15</v>
       </c>
@@ -10384,7 +10392,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="396" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>15</v>
       </c>
@@ -10404,7 +10412,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="397" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>15</v>
       </c>
@@ -10424,7 +10432,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="398" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>14</v>
       </c>
@@ -10444,7 +10452,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="399" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>16</v>
       </c>
@@ -10476,7 +10484,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="400" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>16</v>
       </c>
@@ -10508,7 +10516,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="401" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>16</v>
       </c>
@@ -10540,7 +10548,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="402" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>13</v>
       </c>
@@ -10558,7 +10566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="403" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>15</v>
       </c>
@@ -10578,7 +10586,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="404" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>15</v>
       </c>
@@ -10598,7 +10606,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="405" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>17</v>
       </c>
@@ -10618,7 +10626,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="406" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>14</v>
       </c>
@@ -10638,7 +10646,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="407" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>16</v>
       </c>
@@ -10670,7 +10678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="408" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>16</v>
       </c>
@@ -10702,7 +10710,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="409" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>13</v>
       </c>
@@ -10720,7 +10728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="410" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>15</v>
       </c>
@@ -10740,7 +10748,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="411" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>15</v>
       </c>
@@ -10760,7 +10768,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="412" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>14</v>
       </c>
@@ -10780,7 +10788,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="413" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>16</v>
       </c>
@@ -10812,7 +10820,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="414" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>16</v>
       </c>
@@ -10844,7 +10852,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="415" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>18</v>
       </c>
@@ -10867,7 +10875,7 @@
         <v>8795</v>
       </c>
     </row>
-    <row r="416" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>13</v>
       </c>
@@ -10885,7 +10893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="417" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>15</v>
       </c>
@@ -10905,7 +10913,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="418" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>15</v>
       </c>
@@ -10925,7 +10933,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="419" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>14</v>
       </c>
@@ -10945,7 +10953,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="420" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>16</v>
       </c>
@@ -10977,7 +10985,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="421" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>16</v>
       </c>
@@ -11009,7 +11017,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="422" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>18</v>
       </c>
@@ -11032,7 +11040,7 @@
         <v>8795</v>
       </c>
     </row>
-    <row r="423" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>13</v>
       </c>
@@ -11050,7 +11058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="424" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>15</v>
       </c>
@@ -11070,7 +11078,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="425" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>15</v>
       </c>
@@ -11090,7 +11098,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="426" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>14</v>
       </c>
@@ -11110,7 +11118,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="427" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>16</v>
       </c>
@@ -11142,7 +11150,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="428" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>16</v>
       </c>
@@ -11174,7 +11182,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="429" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>18</v>
       </c>
@@ -11197,7 +11205,7 @@
         <v>8795</v>
       </c>
     </row>
-    <row r="430" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>13</v>
       </c>
@@ -11215,7 +11223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="431" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>15</v>
       </c>
@@ -11235,7 +11243,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="432" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>15</v>
       </c>
@@ -11255,7 +11263,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="433" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>14</v>
       </c>
@@ -11275,7 +11283,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="434" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>16</v>
       </c>
@@ -11307,7 +11315,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="435" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>16</v>
       </c>
@@ -11339,7 +11347,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="436" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
         <v>18</v>
       </c>
@@ -11362,7 +11370,7 @@
         <v>8795</v>
       </c>
     </row>
-    <row r="437" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
         <v>13</v>
       </c>
@@ -11380,7 +11388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="438" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
         <v>15</v>
       </c>
@@ -11400,7 +11408,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="439" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
         <v>15</v>
       </c>
@@ -11420,7 +11428,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="440" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
         <v>14</v>
       </c>
@@ -11440,7 +11448,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="441" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
         <v>16</v>
       </c>
@@ -11472,7 +11480,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="442" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
         <v>16</v>
       </c>
@@ -11504,7 +11512,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="443" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
         <v>13</v>
       </c>
@@ -11522,7 +11530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="444" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
         <v>15</v>
       </c>
@@ -11542,7 +11550,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="445" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
         <v>15</v>
       </c>
@@ -11562,7 +11570,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="446" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
         <v>14</v>
       </c>
@@ -11582,7 +11590,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="447" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
         <v>16</v>
       </c>
@@ -11614,7 +11622,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="448" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
         <v>16</v>
       </c>
@@ -11646,7 +11654,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="449" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
         <v>13</v>
       </c>
@@ -11664,7 +11672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="450" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
         <v>15</v>
       </c>
@@ -11684,7 +11692,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="451" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
         <v>15</v>
       </c>
@@ -11704,7 +11712,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="452" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
         <v>14</v>
       </c>
@@ -11724,7 +11732,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="453" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
         <v>16</v>
       </c>
@@ -11756,7 +11764,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="454" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
         <v>16</v>
       </c>
@@ -11788,7 +11796,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="455" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
         <v>13</v>
       </c>
@@ -11806,7 +11814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="456" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
         <v>15</v>
       </c>
@@ -11826,7 +11834,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="457" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
         <v>15</v>
       </c>
@@ -11846,7 +11854,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="458" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
         <v>14</v>
       </c>
@@ -11866,7 +11874,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="459" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
         <v>16</v>
       </c>
@@ -11898,7 +11906,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="460" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
         <v>16</v>
       </c>
@@ -11930,7 +11938,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="461" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
         <v>13</v>
       </c>
@@ -11948,7 +11956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="462" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
         <v>15</v>
       </c>
@@ -11968,7 +11976,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="463" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
         <v>15</v>
       </c>
@@ -11988,7 +11996,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="464" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
         <v>15</v>
       </c>
@@ -12008,7 +12016,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="465" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
         <v>14</v>
       </c>
@@ -12028,7 +12036,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="466" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
         <v>16</v>
       </c>
@@ -12060,7 +12068,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="467" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
         <v>16</v>
       </c>
@@ -12092,7 +12100,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="468" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
         <v>16</v>
       </c>
@@ -12124,7 +12132,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="469" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
         <v>18</v>
       </c>
@@ -12147,7 +12155,7 @@
         <v>9557</v>
       </c>
     </row>
-    <row r="470" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
         <v>13</v>
       </c>
@@ -12165,7 +12173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="471" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
         <v>15</v>
       </c>
@@ -12185,7 +12193,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="472" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
         <v>15</v>
       </c>
@@ -12205,7 +12213,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="473" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
         <v>14</v>
       </c>
@@ -12225,7 +12233,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="474" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
         <v>16</v>
       </c>
@@ -12257,7 +12265,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="475" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
         <v>16</v>
       </c>
@@ -12289,7 +12297,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="476" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
         <v>13</v>
       </c>
@@ -12310,7 +12318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="477" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
         <v>15</v>
       </c>
@@ -12330,7 +12338,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="478" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
         <v>15</v>
       </c>
@@ -12350,7 +12358,7 @@
         <v>39565</v>
       </c>
     </row>
-    <row r="479" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
         <v>14</v>
       </c>
@@ -12370,7 +12378,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="480" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
         <v>16</v>
       </c>
@@ -12402,7 +12410,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="481" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
         <v>16</v>
       </c>
@@ -12432,6 +12440,148 @@
       </c>
       <c r="O481" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="482" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A482" t="s">
+        <v>13</v>
+      </c>
+      <c r="B482" s="2"/>
+      <c r="C482">
+        <v>1566</v>
+      </c>
+      <c r="D482">
+        <v>1972</v>
+      </c>
+      <c r="L482">
+        <v>1</v>
+      </c>
+      <c r="M482">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="483" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A483" t="s">
+        <v>15</v>
+      </c>
+      <c r="B483">
+        <v>52872</v>
+      </c>
+      <c r="C483">
+        <v>1566</v>
+      </c>
+      <c r="E483">
+        <v>1343916</v>
+      </c>
+      <c r="F483" s="1">
+        <v>39491</v>
+      </c>
+      <c r="G483" s="1">
+        <v>39565</v>
+      </c>
+    </row>
+    <row r="484" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A484" t="s">
+        <v>15</v>
+      </c>
+      <c r="B484">
+        <v>52873</v>
+      </c>
+      <c r="C484">
+        <v>1566</v>
+      </c>
+      <c r="E484">
+        <v>902427</v>
+      </c>
+      <c r="F484" s="1">
+        <v>39491</v>
+      </c>
+      <c r="G484" s="1">
+        <v>39565</v>
+      </c>
+    </row>
+    <row r="485" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A485" t="s">
+        <v>14</v>
+      </c>
+      <c r="B485">
+        <v>135589</v>
+      </c>
+      <c r="C485">
+        <v>1566</v>
+      </c>
+      <c r="F485" s="1">
+        <v>39491</v>
+      </c>
+      <c r="G485" s="1">
+        <v>39565</v>
+      </c>
+      <c r="I485">
+        <v>9201</v>
+      </c>
+    </row>
+    <row r="486" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A486" t="s">
+        <v>16</v>
+      </c>
+      <c r="B486">
+        <v>149567</v>
+      </c>
+      <c r="C486">
+        <v>1566</v>
+      </c>
+      <c r="E486">
+        <v>19076899</v>
+      </c>
+      <c r="F486" s="1">
+        <v>39491</v>
+      </c>
+      <c r="G486" s="1">
+        <v>39565</v>
+      </c>
+      <c r="J486">
+        <v>30</v>
+      </c>
+      <c r="K486">
+        <v>1</v>
+      </c>
+      <c r="N486" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="487" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A487" t="s">
+        <v>16</v>
+      </c>
+      <c r="B487">
+        <v>149568</v>
+      </c>
+      <c r="C487">
+        <v>1566</v>
+      </c>
+      <c r="E487">
+        <v>902430</v>
+      </c>
+      <c r="F487" s="1">
+        <v>39491</v>
+      </c>
+      <c r="G487" s="1">
+        <v>39565</v>
+      </c>
+      <c r="J487">
+        <v>10</v>
+      </c>
+      <c r="K487">
+        <v>30</v>
+      </c>
+      <c r="N487" t="s">
+        <v>23</v>
+      </c>
+      <c r="O487" t="s">
+        <v>25</v>
+      </c>
+      <c r="P487">
+        <v>4184451</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjusted simulated patients. beta first rule now excludes when start dates are equivalent
</commit_message>
<xml_diff>
--- a/patient_addition/data.xlsx
+++ b/patient_addition/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erc53/Github/iDiA_Rules_EC/patient_addition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erc53/Github/iDiA_Rules/patient_addition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BE8B72-1F99-E940-9350-59434D93094B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704D5018-C8C3-3E40-BF28-02CA0D43FFA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="1580" windowWidth="27980" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -963,8 +963,8 @@
   <dimension ref="A1:P487"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <pane ySplit="1" topLeftCell="A470" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E481" activeCellId="1" sqref="F486 E481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3869,7 +3869,7 @@
         <v>19076899</v>
       </c>
       <c r="F117" s="1">
-        <v>39491</v>
+        <v>39492</v>
       </c>
       <c r="G117" s="1">
         <v>39565</v>
@@ -4211,7 +4211,7 @@
         <v>19076899</v>
       </c>
       <c r="F131" s="1">
-        <v>39491</v>
+        <v>39492</v>
       </c>
       <c r="G131" s="1">
         <v>39565</v>
@@ -4869,7 +4869,7 @@
         <v>19076899</v>
       </c>
       <c r="F158" s="1">
-        <v>39491</v>
+        <v>39492</v>
       </c>
       <c r="G158" s="1">
         <v>39565</v>
@@ -5052,7 +5052,7 @@
         <v>19076899</v>
       </c>
       <c r="F165" s="1">
-        <v>39491</v>
+        <v>39492</v>
       </c>
       <c r="G165" s="1">
         <v>39565</v>
@@ -5220,7 +5220,7 @@
         <v>19076899</v>
       </c>
       <c r="F172" s="1">
-        <v>39491</v>
+        <v>39492</v>
       </c>
       <c r="G172" s="1">
         <v>39565</v>
@@ -5423,7 +5423,7 @@
         <v>19076899</v>
       </c>
       <c r="F180" s="1">
-        <v>39491</v>
+        <v>39492</v>
       </c>
       <c r="G180" s="1">
         <v>39565</v>
@@ -7642,7 +7642,7 @@
         <v>19076899</v>
       </c>
       <c r="F269" s="1">
-        <v>39491</v>
+        <v>39492</v>
       </c>
       <c r="G269" s="1">
         <v>39565</v>
@@ -7810,7 +7810,7 @@
         <v>19076899</v>
       </c>
       <c r="F276" s="1">
-        <v>39491</v>
+        <v>39492</v>
       </c>
       <c r="G276" s="1">
         <v>39565</v>
@@ -7978,7 +7978,7 @@
         <v>19076899</v>
       </c>
       <c r="F283" s="1">
-        <v>39491</v>
+        <v>39492</v>
       </c>
       <c r="G283" s="1">
         <v>39565</v>
@@ -12987,7 +12987,7 @@
         <v>19076899</v>
       </c>
       <c r="F486" s="1">
-        <v>39491</v>
+        <v>39492</v>
       </c>
       <c r="G486" s="1">
         <v>39565</v>

</xml_diff>

<commit_message>
updated simulated population for newly implemented rules
Former-commit-id: 13e11a01fb068a06b01d339789f3edceab2d9c8e
</commit_message>
<xml_diff>
--- a/patient_addition/data.xlsx
+++ b/patient_addition/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erc53/Github/iDiA_Rules/patient_addition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C768E1FD-CE01-8D4D-9614-8CA38353E0A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F99AE3-A746-254D-8484-B272C768543A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="460" windowWidth="28020" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -953,8 +953,8 @@
   <dimension ref="A1:O493"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <pane ySplit="1" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O496" sqref="O496"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3146,7 +3146,7 @@
         <v>19104396</v>
       </c>
       <c r="E99" s="1">
-        <v>39491</v>
+        <v>39492</v>
       </c>
       <c r="F99" s="1">
         <v>39565</v>
@@ -3278,7 +3278,7 @@
         <v>19076899</v>
       </c>
       <c r="E105" s="1">
-        <v>39491</v>
+        <v>39492</v>
       </c>
       <c r="F105" s="1">
         <v>39565</v>
@@ -11845,7 +11845,7 @@
         <v>24</v>
       </c>
       <c r="O493">
-        <v>4128794</v>
+        <v>4132161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected a simulated patient data route id for timolol oral
</commit_message>
<xml_diff>
--- a/patient_addition/data.xlsx
+++ b/patient_addition/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erc53/Github/iDiA_Rules/patient_addition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F99AE3-A746-254D-8484-B272C768543A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF4B218-9537-634B-88C6-91AFDC1FB6B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="460" windowWidth="28020" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -954,7 +954,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O496" sqref="O496"/>
+      <selection pane="bottomLeft" activeCell="D477" sqref="D477"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
simulated patient data for new branches. fixed bugs based off simulated data
</commit_message>
<xml_diff>
--- a/patient_addition/data.xlsx
+++ b/patient_addition/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erc53/Github/iDiA_Rules/patient_addition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF4B218-9537-634B-88C6-91AFDC1FB6B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D835E36-13F5-C447-83BE-D0C741D0E9CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="460" windowWidth="28020" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="26">
   <si>
     <t>INSERT_TYPE</t>
   </si>
@@ -950,11 +950,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O493"/>
+  <dimension ref="A1:O511"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D477" sqref="D477"/>
+      <pane ySplit="1" topLeftCell="A494" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L507" sqref="L507"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11846,6 +11846,402 @@
       </c>
       <c r="O493">
         <v>4132161</v>
+      </c>
+    </row>
+    <row r="494" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A494" t="s">
+        <v>12</v>
+      </c>
+      <c r="B494">
+        <v>1568</v>
+      </c>
+      <c r="C494">
+        <v>1960</v>
+      </c>
+      <c r="K494">
+        <v>1</v>
+      </c>
+      <c r="L494">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="495" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A495" t="s">
+        <v>14</v>
+      </c>
+      <c r="B495">
+        <v>1568</v>
+      </c>
+      <c r="D495">
+        <v>1398937</v>
+      </c>
+      <c r="E495" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F495" s="1">
+        <v>39565</v>
+      </c>
+    </row>
+    <row r="496" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A496" t="s">
+        <v>14</v>
+      </c>
+      <c r="B496">
+        <v>1568</v>
+      </c>
+      <c r="D496">
+        <v>902427</v>
+      </c>
+      <c r="E496" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F496" s="1">
+        <v>39565</v>
+      </c>
+    </row>
+    <row r="497" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A497" t="s">
+        <v>13</v>
+      </c>
+      <c r="B497">
+        <v>1568</v>
+      </c>
+      <c r="E497" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F497" s="1">
+        <v>39565</v>
+      </c>
+      <c r="H497">
+        <v>9201</v>
+      </c>
+    </row>
+    <row r="498" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A498" t="s">
+        <v>15</v>
+      </c>
+      <c r="B498">
+        <v>1568</v>
+      </c>
+      <c r="D498">
+        <v>40223504</v>
+      </c>
+      <c r="E498" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F498" s="1">
+        <v>39565</v>
+      </c>
+      <c r="I498">
+        <v>30</v>
+      </c>
+      <c r="J498">
+        <v>30</v>
+      </c>
+      <c r="M498" t="s">
+        <v>21</v>
+      </c>
+      <c r="N498" t="s">
+        <v>24</v>
+      </c>
+      <c r="O498" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="499" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A499" t="s">
+        <v>15</v>
+      </c>
+      <c r="B499">
+        <v>1568</v>
+      </c>
+      <c r="D499">
+        <v>1594707</v>
+      </c>
+      <c r="E499" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F499" s="1">
+        <v>39565</v>
+      </c>
+      <c r="I499">
+        <v>30</v>
+      </c>
+      <c r="J499">
+        <v>30</v>
+      </c>
+      <c r="M499" t="s">
+        <v>21</v>
+      </c>
+      <c r="N499" t="s">
+        <v>24</v>
+      </c>
+      <c r="O499" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="500" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A500" t="s">
+        <v>12</v>
+      </c>
+      <c r="B500">
+        <v>1569</v>
+      </c>
+      <c r="C500">
+        <v>1966</v>
+      </c>
+      <c r="K500">
+        <v>1</v>
+      </c>
+      <c r="L500">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="501" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A501" t="s">
+        <v>14</v>
+      </c>
+      <c r="B501">
+        <v>1569</v>
+      </c>
+      <c r="D501">
+        <v>1398937</v>
+      </c>
+      <c r="E501" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F501" s="1">
+        <v>39565</v>
+      </c>
+    </row>
+    <row r="502" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A502" t="s">
+        <v>14</v>
+      </c>
+      <c r="B502">
+        <v>1569</v>
+      </c>
+      <c r="D502">
+        <v>902427</v>
+      </c>
+      <c r="E502" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F502" s="1">
+        <v>39565</v>
+      </c>
+    </row>
+    <row r="503" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A503" t="s">
+        <v>13</v>
+      </c>
+      <c r="B503">
+        <v>1569</v>
+      </c>
+      <c r="E503" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F503" s="1">
+        <v>39565</v>
+      </c>
+      <c r="H503">
+        <v>9201</v>
+      </c>
+    </row>
+    <row r="504" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A504" t="s">
+        <v>15</v>
+      </c>
+      <c r="B504">
+        <v>1569</v>
+      </c>
+      <c r="D504">
+        <v>19079775</v>
+      </c>
+      <c r="E504" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F504" s="1">
+        <v>39565</v>
+      </c>
+      <c r="I504">
+        <v>20</v>
+      </c>
+      <c r="J504">
+        <v>30</v>
+      </c>
+      <c r="M504" t="s">
+        <v>23</v>
+      </c>
+      <c r="N504" t="s">
+        <v>24</v>
+      </c>
+      <c r="O504" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="505" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A505" t="s">
+        <v>15</v>
+      </c>
+      <c r="B505">
+        <v>1569</v>
+      </c>
+      <c r="D505">
+        <v>902489</v>
+      </c>
+      <c r="E505" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F505" s="1">
+        <v>39565</v>
+      </c>
+      <c r="I505">
+        <v>5</v>
+      </c>
+      <c r="J505">
+        <v>30</v>
+      </c>
+      <c r="M505" t="s">
+        <v>23</v>
+      </c>
+      <c r="N505" t="s">
+        <v>24</v>
+      </c>
+      <c r="O505" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="506" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A506" t="s">
+        <v>12</v>
+      </c>
+      <c r="B506">
+        <v>1570</v>
+      </c>
+      <c r="C506">
+        <v>1950</v>
+      </c>
+      <c r="K506">
+        <v>1</v>
+      </c>
+      <c r="L506">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="507" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A507" t="s">
+        <v>14</v>
+      </c>
+      <c r="B507">
+        <v>1570</v>
+      </c>
+      <c r="D507">
+        <v>1398937</v>
+      </c>
+      <c r="E507" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F507" s="1">
+        <v>39565</v>
+      </c>
+    </row>
+    <row r="508" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A508" t="s">
+        <v>14</v>
+      </c>
+      <c r="B508">
+        <v>1570</v>
+      </c>
+      <c r="D508">
+        <v>950370</v>
+      </c>
+      <c r="E508" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F508" s="1">
+        <v>39565</v>
+      </c>
+    </row>
+    <row r="509" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A509" t="s">
+        <v>13</v>
+      </c>
+      <c r="B509">
+        <v>1570</v>
+      </c>
+      <c r="E509" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F509" s="1">
+        <v>39565</v>
+      </c>
+      <c r="H509">
+        <v>9201</v>
+      </c>
+    </row>
+    <row r="510" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A510" t="s">
+        <v>15</v>
+      </c>
+      <c r="B510">
+        <v>1570</v>
+      </c>
+      <c r="D510">
+        <v>40223506</v>
+      </c>
+      <c r="E510" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F510" s="1">
+        <v>39565</v>
+      </c>
+      <c r="I510">
+        <v>10</v>
+      </c>
+      <c r="J510">
+        <v>10</v>
+      </c>
+      <c r="M510" t="s">
+        <v>20</v>
+      </c>
+      <c r="N510" t="s">
+        <v>24</v>
+      </c>
+      <c r="O510" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="511" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A511" t="s">
+        <v>15</v>
+      </c>
+      <c r="B511">
+        <v>1570</v>
+      </c>
+      <c r="D511">
+        <v>43219718</v>
+      </c>
+      <c r="E511" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F511" s="1">
+        <v>39565</v>
+      </c>
+      <c r="I511">
+        <v>30</v>
+      </c>
+      <c r="J511">
+        <v>30</v>
+      </c>
+      <c r="M511" t="s">
+        <v>21</v>
+      </c>
+      <c r="N511" t="s">
+        <v>24</v>
+      </c>
+      <c r="O511" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simulated patient for ceftriaxone calcium
Former-commit-id: 0c7c3df32d124f1ad04028331f722ffed36e1a7f
</commit_message>
<xml_diff>
--- a/patient_addition/data.xlsx
+++ b/patient_addition/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erc53/Github/iDiA_Rules/patient_addition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D835E36-13F5-C447-83BE-D0C741D0E9CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7A6693-A305-DE45-9C89-AFE01B3597DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="28020" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="460" windowWidth="28000" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="26">
   <si>
     <t>INSERT_TYPE</t>
   </si>
@@ -950,11 +950,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O511"/>
+  <dimension ref="A1:O517"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A494" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L507" sqref="L507"/>
+      <selection pane="bottomLeft" activeCell="G514" sqref="G514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12241,6 +12241,138 @@
         <v>24</v>
       </c>
       <c r="O511" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="512" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A512" t="s">
+        <v>12</v>
+      </c>
+      <c r="B512">
+        <v>1571</v>
+      </c>
+      <c r="C512">
+        <v>1950</v>
+      </c>
+      <c r="K512">
+        <v>1</v>
+      </c>
+      <c r="L512">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A513" t="s">
+        <v>14</v>
+      </c>
+      <c r="B513">
+        <v>1571</v>
+      </c>
+      <c r="D513">
+        <v>19036781</v>
+      </c>
+      <c r="E513" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F513" s="1">
+        <v>39565</v>
+      </c>
+    </row>
+    <row r="514" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A514" t="s">
+        <v>14</v>
+      </c>
+      <c r="B514">
+        <v>1571</v>
+      </c>
+      <c r="D514">
+        <v>1777806</v>
+      </c>
+      <c r="E514" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F514" s="1">
+        <v>39565</v>
+      </c>
+    </row>
+    <row r="515" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A515" t="s">
+        <v>13</v>
+      </c>
+      <c r="B515">
+        <v>1571</v>
+      </c>
+      <c r="E515" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F515" s="1">
+        <v>39565</v>
+      </c>
+      <c r="H515">
+        <v>9201</v>
+      </c>
+    </row>
+    <row r="516" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A516" t="s">
+        <v>15</v>
+      </c>
+      <c r="B516">
+        <v>1571</v>
+      </c>
+      <c r="D516">
+        <v>45775952</v>
+      </c>
+      <c r="E516" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F516" s="1">
+        <v>39565</v>
+      </c>
+      <c r="I516">
+        <v>10</v>
+      </c>
+      <c r="J516">
+        <v>10</v>
+      </c>
+      <c r="M516" t="s">
+        <v>20</v>
+      </c>
+      <c r="N516" t="s">
+        <v>24</v>
+      </c>
+      <c r="O516" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="517" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A517" t="s">
+        <v>15</v>
+      </c>
+      <c r="B517">
+        <v>1571</v>
+      </c>
+      <c r="D517">
+        <v>46287321</v>
+      </c>
+      <c r="E517" s="1">
+        <v>39491</v>
+      </c>
+      <c r="F517" s="1">
+        <v>39565</v>
+      </c>
+      <c r="I517">
+        <v>1</v>
+      </c>
+      <c r="J517">
+        <v>1</v>
+      </c>
+      <c r="M517" t="s">
+        <v>20</v>
+      </c>
+      <c r="N517" t="s">
+        <v>24</v>
+      </c>
+      <c r="O517" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
epinephrine dosage adjustments in simulated data
</commit_message>
<xml_diff>
--- a/patient_addition/data.xlsx
+++ b/patient_addition/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erc53/Github/iDiA_Rules/patient_addition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7A6693-A305-DE45-9C89-AFE01B3597DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3946E55-D62A-134D-8494-B1965A9F2D3E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="800" yWindow="460" windowWidth="28000" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -953,8 +953,8 @@
   <dimension ref="A1:O517"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A494" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G514" sqref="G514"/>
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K145" sqref="K145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3995,7 +3995,7 @@
         <v>1514</v>
       </c>
       <c r="D138">
-        <v>19076899</v>
+        <v>40226826</v>
       </c>
       <c r="E138" s="1">
         <v>39491</v>
@@ -4004,7 +4004,7 @@
         <v>39565</v>
       </c>
       <c r="I138">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="J138">
         <v>1</v>
@@ -7049,7 +7049,7 @@
         <v>1534</v>
       </c>
       <c r="D276">
-        <v>19076899</v>
+        <v>19127146</v>
       </c>
       <c r="E276" s="1">
         <v>39492</v>
@@ -7058,13 +7058,13 @@
         <v>39565</v>
       </c>
       <c r="I276">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J276">
         <v>1</v>
       </c>
       <c r="M276" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N276" t="s">
         <v>24</v>
@@ -11792,7 +11792,7 @@
         <v>1567</v>
       </c>
       <c r="D492">
-        <v>19076899</v>
+        <v>19127146</v>
       </c>
       <c r="E492" s="1">
         <v>39492</v>
@@ -11801,13 +11801,13 @@
         <v>39565</v>
       </c>
       <c r="I492">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="J492">
         <v>1</v>
       </c>
       <c r="M492" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N492" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
simulated patient for testing alternative basic concomitant timeline
</commit_message>
<xml_diff>
--- a/patient_addition/data.xlsx
+++ b/patient_addition/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erc53/Github/iDiA_Rules/patient_addition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F10901-B72D-8E4A-A802-7AD4FBE2261F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DF89C7-AFE3-AC43-B5CF-397863174A16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="800" yWindow="460" windowWidth="28000" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -950,8 +950,8 @@
   <dimension ref="A1:N526"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A498" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D521" sqref="D521"/>
+      <pane ySplit="1" topLeftCell="A366" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E375" sqref="E375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8861,7 +8861,7 @@
         <v>1307046</v>
       </c>
       <c r="E375" s="1">
-        <v>39491</v>
+        <v>39492</v>
       </c>
       <c r="F375" s="1">
         <v>39565</v>
@@ -8941,7 +8941,7 @@
         <v>46221724</v>
       </c>
       <c r="E379" s="1">
-        <v>39491</v>
+        <v>39492</v>
       </c>
       <c r="F379" s="1">
         <v>39565</v>

</xml_diff>